<commit_message>
work on orange operator
</commit_message>
<xml_diff>
--- a/Lamia/DBASE/create/Base2_chantiertram_0_1.xlsx
+++ b/Lamia/DBASE/create/Base2_chantiertram_0_1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrice.verchere\PycharmProjects\Lamia\Lamia\DBASE\create\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AAC906-1EC6-458C-BBD3-AF5AE0126D72}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="3"/>
+    <workbookView xWindow="2640" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="767" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="18" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="04_Observation" sheetId="21" r:id="rId4"/>
     <sheet name="02_Intervenant" sheetId="22" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateCount="1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="389">
   <si>
     <t>00_Basedonnees'!A1</t>
   </si>
@@ -770,19 +776,453 @@
   </si>
   <si>
     <t>lid_ressource_entocc</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Contrôle</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>commune</t>
+  </si>
+  <si>
+    <t>rue</t>
+  </si>
+  <si>
+    <t>datedebuttravaux</t>
+  </si>
+  <si>
+    <t>datefincontractuelle</t>
+  </si>
+  <si>
+    <t>#**************** TRAM</t>
+  </si>
+  <si>
+    <t>#**************** ORANGE</t>
+  </si>
+  <si>
+    <t>#****** calendrier</t>
+  </si>
+  <si>
+    <t>#******* effectifs</t>
+  </si>
+  <si>
+    <t>#*****ENGINS</t>
+  </si>
+  <si>
+    <t>#***** SECURITE</t>
+  </si>
+  <si>
+    <t>#**************** NCA *************************************</t>
+  </si>
+  <si>
+    <t># ****** TRAM</t>
+  </si>
+  <si>
+    <t>#**************** NCB *************************************</t>
+  </si>
+  <si>
+    <t>#divers</t>
+  </si>
+  <si>
+    <t>za_sro</t>
+  </si>
+  <si>
+    <t># ****** ORANGE</t>
+  </si>
+  <si>
+    <t>nca_meteo</t>
+  </si>
+  <si>
+    <t>nca_etp_presentes</t>
+  </si>
+  <si>
+    <t>nca_planning</t>
+  </si>
+  <si>
+    <t>nca_planning_com</t>
+  </si>
+  <si>
+    <t>nca_effectif_entreprise</t>
+  </si>
+  <si>
+    <t>nca_effectif_sstraitant</t>
+  </si>
+  <si>
+    <t>nca_engins_pelle</t>
+  </si>
+  <si>
+    <t>nca_engins_chargeuse</t>
+  </si>
+  <si>
+    <t>nca_engins_compresseur</t>
+  </si>
+  <si>
+    <t>nca_engins_trancheuse</t>
+  </si>
+  <si>
+    <t>nca_engins_camionsmat</t>
+  </si>
+  <si>
+    <t>nca_engins_camiondeb</t>
+  </si>
+  <si>
+    <t>nca_engins_camionasp</t>
+  </si>
+  <si>
+    <t>nca_engins_camionrep</t>
+  </si>
+  <si>
+    <t>nca_engins_camionmal</t>
+  </si>
+  <si>
+    <t>nca_engins_container</t>
+  </si>
+  <si>
+    <t>nca_engins_compacteur</t>
+  </si>
+  <si>
+    <t>nca_engins_finisseur</t>
+  </si>
+  <si>
+    <t>nca_engins_minipelle</t>
+  </si>
+  <si>
+    <t>nca_engins_nacelle</t>
+  </si>
+  <si>
+    <t>nca_engins_autres</t>
+  </si>
+  <si>
+    <t>nca_sec_personnel</t>
+  </si>
+  <si>
+    <t>nca_sec_protection</t>
+  </si>
+  <si>
+    <t>nca_sec_afficharrete</t>
+  </si>
+  <si>
+    <t>nca_sec_panneauxchant</t>
+  </si>
+  <si>
+    <t>nca_sec_circul</t>
+  </si>
+  <si>
+    <t>nca_sec_eclairage</t>
+  </si>
+  <si>
+    <t>nca_sec_stockagedechet</t>
+  </si>
+  <si>
+    <t>nca_sec_proprete</t>
+  </si>
+  <si>
+    <t>nca_sec_protectiontranchee</t>
+  </si>
+  <si>
+    <t>nca_sec_blindage</t>
+  </si>
+  <si>
+    <t>nca_sec_reunionmarquage</t>
+  </si>
+  <si>
+    <t>nca_sec_entretienmarquage</t>
+  </si>
+  <si>
+    <t>nca_sec_accesscoupure</t>
+  </si>
+  <si>
+    <t>nca_sec_travailhauteur</t>
+  </si>
+  <si>
+    <t>nca_sec_plaintes</t>
+  </si>
+  <si>
+    <t>nca_sec_plaintes_com</t>
+  </si>
+  <si>
+    <t>nca_conducteurdetravaux</t>
+  </si>
+  <si>
+    <t>lid_observation</t>
+  </si>
+  <si>
+    <t>#**************** sousfiche  *************************************</t>
+  </si>
+  <si>
+    <t>code_sro</t>
+  </si>
+  <si>
+    <t>item_type_1</t>
+  </si>
+  <si>
+    <t>item_obs_1</t>
+  </si>
+  <si>
+    <t>item_type_2</t>
+  </si>
+  <si>
+    <t>item_obs_3</t>
+  </si>
+  <si>
+    <t>item_obs_2</t>
+  </si>
+  <si>
+    <t>item_type_3</t>
+  </si>
+  <si>
+    <t>item_type_4</t>
+  </si>
+  <si>
+    <t>item_obs_4</t>
+  </si>
+  <si>
+    <t>item_type_5</t>
+  </si>
+  <si>
+    <t>item_obs_5</t>
+  </si>
+  <si>
+    <t>item_type_6</t>
+  </si>
+  <si>
+    <t>item_obs_6</t>
+  </si>
+  <si>
+    <t>item_type_7</t>
+  </si>
+  <si>
+    <t>item_obs_7</t>
+  </si>
+  <si>
+    <t>item_type_8</t>
+  </si>
+  <si>
+    <t>item_obs_8</t>
+  </si>
+  <si>
+    <t>item_type_9</t>
+  </si>
+  <si>
+    <t>item_obs_9</t>
+  </si>
+  <si>
+    <t>item_type_10</t>
+  </si>
+  <si>
+    <t>item_obs_10</t>
+  </si>
+  <si>
+    <t>item_type_11</t>
+  </si>
+  <si>
+    <t>item_obs_11</t>
+  </si>
+  <si>
+    <t>item_type_12</t>
+  </si>
+  <si>
+    <t>item_obs_12</t>
+  </si>
+  <si>
+    <t>item_type_13</t>
+  </si>
+  <si>
+    <t>item_obs_13</t>
+  </si>
+  <si>
+    <t>item_type_14</t>
+  </si>
+  <si>
+    <t>item_obs_14</t>
+  </si>
+  <si>
+    <t>item_type_15</t>
+  </si>
+  <si>
+    <t>item_obs_15</t>
+  </si>
+  <si>
+    <t>item_type_16</t>
+  </si>
+  <si>
+    <t>item_obs_16</t>
+  </si>
+  <si>
+    <t>item_type_17</t>
+  </si>
+  <si>
+    <t>item_obs_17</t>
+  </si>
+  <si>
+    <t>item_type_18</t>
+  </si>
+  <si>
+    <t>item_obs_18</t>
+  </si>
+  <si>
+    <t>item_type_19</t>
+  </si>
+  <si>
+    <t>item_obs_19</t>
+  </si>
+  <si>
+    <t>item_type_20</t>
+  </si>
+  <si>
+    <t>item_obs_20</t>
+  </si>
+  <si>
+    <t>item_type_21</t>
+  </si>
+  <si>
+    <t>item_obs_21</t>
+  </si>
+  <si>
+    <t>item_type_22</t>
+  </si>
+  <si>
+    <t>item_obs_22</t>
+  </si>
+  <si>
+    <t>item_type_23</t>
+  </si>
+  <si>
+    <t>item_obs_23</t>
+  </si>
+  <si>
+    <t>item_type_24</t>
+  </si>
+  <si>
+    <t>item_obs_24</t>
+  </si>
+  <si>
+    <t>item_type_25</t>
+  </si>
+  <si>
+    <t>item_obs_25</t>
+  </si>
+  <si>
+    <t>item_type_26</t>
+  </si>
+  <si>
+    <t>item_obs_26</t>
+  </si>
+  <si>
+    <t>item_type_27</t>
+  </si>
+  <si>
+    <t>item_obs_27</t>
+  </si>
+  <si>
+    <t>item_type_28</t>
+  </si>
+  <si>
+    <t>item_obs_28</t>
+  </si>
+  <si>
+    <t>item_type_29</t>
+  </si>
+  <si>
+    <t>item_obs_29</t>
+  </si>
+  <si>
+    <t>item_type_30</t>
+  </si>
+  <si>
+    <t>item_obs_30</t>
+  </si>
+  <si>
+    <t>item_type_31</t>
+  </si>
+  <si>
+    <t>item_obs_31</t>
+  </si>
+  <si>
+    <t>item_type_32</t>
+  </si>
+  <si>
+    <t>item_obs_32</t>
+  </si>
+  <si>
+    <t>item_type_33</t>
+  </si>
+  <si>
+    <t>item_obs_33</t>
+  </si>
+  <si>
+    <t>item_type_34</t>
+  </si>
+  <si>
+    <t>item_obs_34</t>
+  </si>
+  <si>
+    <t>item_type_35</t>
+  </si>
+  <si>
+    <t>item_obs_35</t>
+  </si>
+  <si>
+    <t>item_type_36</t>
+  </si>
+  <si>
+    <t>item_obs_36</t>
+  </si>
+  <si>
+    <t>item_type_37</t>
+  </si>
+  <si>
+    <t>item_obs_37</t>
+  </si>
+  <si>
+    <t>item_type_38</t>
+  </si>
+  <si>
+    <t>item_obs_38</t>
+  </si>
+  <si>
+    <t>item_type_39</t>
+  </si>
+  <si>
+    <t>item_obs_39</t>
+  </si>
+  <si>
+    <t>item_type_40</t>
+  </si>
+  <si>
+    <t>item_obs_40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -903,50 +1343,56 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -995,7 +1441,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1028,9 +1474,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1063,6 +1526,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1238,7 +1718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -1629,60 +2109,60 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1"/>
-    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1"/>
-    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1"/>
-    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1"/>
-    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1"/>
-    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1"/>
-    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1"/>
-    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1"/>
-    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1"/>
-    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1"/>
-    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1"/>
-    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1"/>
-    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1"/>
-    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1"/>
-    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1"/>
-    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1"/>
-    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1"/>
-    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1"/>
-    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1"/>
-    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1"/>
-    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1"/>
-    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1"/>
-    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1"/>
-    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1"/>
-    <hyperlink ref="B25" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1"/>
-    <hyperlink ref="B26" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1"/>
-    <hyperlink ref="B27" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1"/>
-    <hyperlink ref="B28" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1"/>
-    <hyperlink ref="B29" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1"/>
-    <hyperlink ref="B30" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1"/>
-    <hyperlink ref="B31" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1"/>
-    <hyperlink ref="B32" location="'10_auth_group'!A1" display="'10_auth_group'!A1"/>
-    <hyperlink ref="B33" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1"/>
-    <hyperlink ref="B34" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1"/>
-    <hyperlink ref="B35" location="'10_auth_user'!A1" display="'10_auth_user'!A1"/>
-    <hyperlink ref="B36" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1"/>
-    <hyperlink ref="B37" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1"/>
-    <hyperlink ref="B38" location="'10_bdd'!A1" display="'10_bdd'!A1"/>
-    <hyperlink ref="B39" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1"/>
-    <hyperlink ref="B40" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1"/>
-    <hyperlink ref="B41" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1"/>
-    <hyperlink ref="B42" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1"/>
-    <hyperlink ref="B43" location="'10_django_session'!A1" display="'10_django_session'!A1"/>
-    <hyperlink ref="B44" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1"/>
-    <hyperlink ref="B45" location="'10_projet'!A1" display="'10_projet'!A1"/>
-    <hyperlink ref="B46" location="'10_siartelia'!A1" display="'10_siartelia'!A1"/>
-    <hyperlink ref="B47" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1"/>
+    <hyperlink ref="B1" location="'00_Basedonnees'!A1" display="'00_Basedonnees'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" location="'00_Revision'!A1" display="'00_Revision'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B3" location="'01_Objet'!A1" display="'01_Objet'!A1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B4" location="'02_Descriptionsystem'!A1" display="'02_Descriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" location="'02_Evenement'!A1" display="'02_Evenement'!A1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B6" location="'02_Marche'!A1" display="'02_Marche'!A1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" location="'02_Zonegeo'!A1" display="'02_Zonegeo'!A1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" location="'03_Desordre'!A1" display="'03_Desordre'!A1" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" location="'03_Interventiontiers'!A1" display="'03_Interventiontiers'!A1" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B10" location="'03_Ressource'!A1" display="'03_Ressource'!A1" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B11" location="'04_Infralineaire'!A1" display="'04_Infralineaire'!A1" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B12" location="'04_Environnement'!A1" display="'04_Environnement'!A1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B13" location="'04_Equipement'!A1" display="'04_Equipement'!A1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B14" location="'04_Etudestrategie'!A1" display="'04_Etudestrategie'!A1" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B15" location="'04_Noeud'!A1" display="'04_Noeud'!A1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B16" location="'04_Observation'!A1" display="'04_Observation'!A1" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B17" location="'04_Profil'!A1" display="'04_Profil'!A1" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B18" location="'05_Graphique'!A1" display="'05_Graphique'!A1" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B19" location="'05_Modele'!A1" display="'05_Modele'!A1" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B20" location="'05_Photo'!A1" display="'05_Photo'!A1" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B21" location="'05_Rapport'!A1" display="'05_Rapport'!A1" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B22" location="'05_Rasters'!A1" display="'05_Rasters'!A1" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B23" location="'05_Topographie'!A1" display="'05_Topographie'!A1" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B24" location="'05_Travaux'!A1" display="'05_Travaux'!A1" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B25" location="'06_Graphiquedata'!A1" display="'06_Graphiquedata'!A1" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B26" location="'06_Pointtopo'!A1" display="'06_Pointtopo'!A1" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B27" location="'06_Tcetudetravaux'!A1" display="'06_Tcetudetravaux'!A1" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B28" location="'06_Tcobjetintervenant'!A1" display="'06_Tcobjetintervenant'!A1" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B29" location="'06_Tcobjetressource'!A1" display="'06_Tcobjetressource'!A1" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B30" location="'06_Tcobjetzonegeo'!A1" display="'06_Tcobjetzonegeo'!A1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B31" location="'06_Tctravauxdescriptionsystem'!A1" display="'06_Tctravauxdescriptionsystem'!A1" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B32" location="'10_auth_group'!A1" display="'10_auth_group'!A1" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B33" location="'10_auth_group_permissions'!A1" display="'10_auth_group_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B34" location="'10_auth_permission'!A1" display="'10_auth_permission'!A1" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B35" location="'10_auth_user'!A1" display="'10_auth_user'!A1" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B36" location="'10_auth_user_groups'!A1" display="'10_auth_user_groups'!A1" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B37" location="'10_auth_user_user_permissions'!A1" display="'10_auth_user_user_permissions'!A1" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B38" location="'10_bdd'!A1" display="'10_bdd'!A1" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B39" location="'10_carto_layer'!A1" display="'10_carto_layer'!A1" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B40" location="'10_django_admin_log'!A1" display="'10_django_admin_log'!A1" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B41" location="'10_django_content_type'!A1" display="'10_django_content_type'!A1" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B42" location="'10_django_migrations'!A1" display="'10_django_migrations'!A1" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B43" location="'10_django_session'!A1" display="'10_django_session'!A1" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B44" location="'10_messagetiers'!A1" display="'10_messagetiers'!A1" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B45" location="'10_projet'!A1" display="'10_projet'!A1" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B46" location="'10_siartelia'!A1" display="'10_siartelia'!A1" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B47" location="'11_utilisateur'!A1" display="'11_utilisateur'!A1" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1786,22 +2266,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="21.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="3" customWidth="1"/>
+    <col min="2" max="3" width="21.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="52.85546875" style="3" customWidth="1"/>
     <col min="5" max="7" width="21.85546875" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="11.42578125" style="3"/>
+    <col min="8" max="8" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>222</v>
       </c>
@@ -1810,7 +2294,7 @@
       </c>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1818,8 +2302,11 @@
       <c r="F2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -1844,8 +2331,17 @@
       <c r="H3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -1856,7 +2352,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1867,7 +2363,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>110</v>
       </c>
@@ -1881,7 +2377,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>117</v>
       </c>
@@ -1897,8 +2393,14 @@
       <c r="G8" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="J8" s="19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F9" s="17" t="s">
         <v>167</v>
       </c>
@@ -1906,7 +2408,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>120</v>
       </c>
@@ -1914,7 +2416,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>121</v>
       </c>
@@ -1922,7 +2424,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>122</v>
       </c>
@@ -1930,7 +2432,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>123</v>
       </c>
@@ -1950,8 +2452,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>169</v>
+      <c r="A19" s="20" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2005,17 +2507,75 @@
         <v>108</v>
       </c>
     </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="B33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2658,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="20" t="s">
         <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2258,13 +2818,21 @@
         <v>108</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="20" t="s">
         <v>170</v>
       </c>
       <c r="B29" t="s">
@@ -2318,40 +2886,34 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="B37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
         <v>108</v>
@@ -2359,7 +2921,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B40" t="s">
         <v>108</v>
@@ -2367,7 +2929,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
         <v>108</v>
@@ -2375,7 +2937,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B42" t="s">
         <v>108</v>
@@ -2383,448 +2945,1824 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B43" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="F44" s="8" t="s">
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="F47" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45"/>
-      <c r="F45" s="7" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48"/>
+      <c r="F48" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="G45" s="7">
+      <c r="G48" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46"/>
-      <c r="F46" s="7" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49"/>
+      <c r="F49" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="G46" s="3">
+      <c r="G49" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47"/>
-      <c r="F47" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="G47" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="B48" t="s">
-        <v>118</v>
-      </c>
-      <c r="F48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="B49" t="s">
-        <v>118</v>
-      </c>
-      <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50"/>
-      <c r="F50" s="7"/>
+      <c r="F50" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G50" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51"/>
+      <c r="A51" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
+      <c r="A52" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B53"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B58" t="s">
+        <v>108</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="19"/>
+      <c r="B59"/>
+      <c r="F59" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="19"/>
+      <c r="B60"/>
+      <c r="F60" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G60" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+      <c r="B62"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B65" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="B66" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B69" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B70" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="B73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B74" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B77" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B79" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="B83" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="20"/>
+      <c r="B87" s="20"/>
+      <c r="F87" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G87" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="F88" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G88" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="20"/>
+      <c r="F90" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G90" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="20"/>
+      <c r="F91" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G91" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F92" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="20"/>
+      <c r="F93" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G93" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="20"/>
+      <c r="F94" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G94" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="20"/>
+      <c r="F96" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G96" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="20"/>
+      <c r="F97" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G97" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F98" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="20"/>
+      <c r="F99" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G99" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
+      <c r="F100" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G100" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="20"/>
+      <c r="F102" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G102" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="20"/>
+      <c r="F103" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G103" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="F105" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G105" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="20"/>
+      <c r="F106" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G106" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="20"/>
+      <c r="F108" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G108" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="20"/>
+      <c r="F109" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G109" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F110" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="20"/>
+      <c r="F111" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G111" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="20"/>
+      <c r="F112" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G112" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F113" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
+      <c r="F114" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G114" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
+      <c r="F115" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G115" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F116" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="F117" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G117" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="F118" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G118" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F119" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="F120" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G120" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="20"/>
+      <c r="F121" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G121" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F122" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="20"/>
+      <c r="F123" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G123" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="20"/>
+      <c r="F124" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G124" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F125" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="20"/>
+      <c r="F126" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G126" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="20"/>
+      <c r="F127" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G127" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B128" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F128" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="F129" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="G129" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F130" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G130" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B131" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="7"/>
+      <c r="B132"/>
+      <c r="F132" s="7"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B53" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="7" t="s">
+      <c r="B134" t="s">
+        <v>108</v>
+      </c>
+      <c r="D134" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B54" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="7" t="s">
+      <c r="B135" t="s">
+        <v>108</v>
+      </c>
+      <c r="D135" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B136" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D55" s="7"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B56" t="s">
-        <v>108</v>
-      </c>
-      <c r="D56" s="12" t="s">
+      <c r="B137" t="s">
+        <v>108</v>
+      </c>
+      <c r="D137" s="12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="B57" t="s">
-        <v>108</v>
-      </c>
-      <c r="D57" s="7" t="s">
+      <c r="B138" t="s">
+        <v>108</v>
+      </c>
+      <c r="D138" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B139" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B59" t="s">
-        <v>108</v>
-      </c>
-      <c r="D59" s="7" t="s">
+      <c r="B140" t="s">
+        <v>108</v>
+      </c>
+      <c r="D140" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="B60" t="s">
-        <v>108</v>
-      </c>
-      <c r="D60" s="7" t="s">
+      <c r="B141" t="s">
+        <v>108</v>
+      </c>
+      <c r="D141" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="12" t="s">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B142" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="12"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="12"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="12"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="12"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="12"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="B63" t="s">
-        <v>108</v>
-      </c>
-      <c r="F63" s="11" t="s">
+      <c r="B149" t="s">
+        <v>108</v>
+      </c>
+      <c r="F149" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G149" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F64" s="10" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F150" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G150" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F65" s="10" t="s">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F151" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G151" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="16" t="s">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="B68" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+      <c r="B154" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="B69" t="s">
-        <v>108</v>
-      </c>
-      <c r="D69" s="10" t="s">
+      <c r="B155" t="s">
+        <v>108</v>
+      </c>
+      <c r="D155" s="10" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="B71" t="s">
-        <v>108</v>
-      </c>
-      <c r="F71" s="11" t="s">
+      <c r="B157" t="s">
+        <v>108</v>
+      </c>
+      <c r="F157" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="G71" s="3">
+      <c r="G157" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F72" s="10" t="s">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F158" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="G72" s="3">
+      <c r="G158" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F73" s="10" t="s">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F159" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="G73" s="3">
+      <c r="G159" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="B74" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="16" t="s">
+      <c r="B160" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B161" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
-      <c r="B76"/>
-      <c r="D76" s="7"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="10"/>
+      <c r="B162"/>
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B77" t="s">
-        <v>108</v>
-      </c>
-      <c r="D77" s="7"/>
-      <c r="F77" s="13" t="s">
+      <c r="B163" t="s">
+        <v>108</v>
+      </c>
+      <c r="D163" s="7"/>
+      <c r="F163" s="13" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78"/>
-      <c r="D78" s="7"/>
-      <c r="F78" s="12" t="s">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="12"/>
+      <c r="B164"/>
+      <c r="D164" s="7"/>
+      <c r="F164" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="G78" s="3">
+      <c r="G164" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79"/>
-      <c r="D79" s="7"/>
-      <c r="F79" s="12" t="s">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="12"/>
+      <c r="B165"/>
+      <c r="D165" s="7"/>
+      <c r="F165" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="G79" s="3">
+      <c r="G165" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
-      <c r="B80"/>
-      <c r="D80" s="7"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="12"/>
+      <c r="B166"/>
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="B81" t="s">
-        <v>118</v>
-      </c>
-      <c r="D81" s="7"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="16" t="s">
+      <c r="B167" t="s">
+        <v>118</v>
+      </c>
+      <c r="D167" s="7"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="B83" t="s">
-        <v>108</v>
-      </c>
-      <c r="F83" s="13" t="s">
+      <c r="B169" t="s">
+        <v>108</v>
+      </c>
+      <c r="F169" s="13" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F84" s="12" t="s">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F170" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="G84" s="3">
+      <c r="G170" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F85" s="12" t="s">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F171" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="G85" s="3">
+      <c r="G171" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="16" t="s">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="16" t="s">
         <v>231</v>
       </c>
-      <c r="B86" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="B172" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B175" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="B90" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
+      <c r="B176" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B92" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
+      <c r="B178" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="B93" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+      <c r="B179" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="B94" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
+      <c r="B180" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B181" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="B97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
+      <c r="B183" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="B98" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
+      <c r="B184" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="B99" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
+      <c r="B185" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B186" s="3" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="20" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="B189" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B191" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B192" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B193" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="B194" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B195" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B196" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="B197" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="B198" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="B199" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B200" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="B201" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B202" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="B203" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="B204" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="B205" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="20" t="s">
+        <v>324</v>
+      </c>
+      <c r="B206" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="B207" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="20" t="s">
+        <v>326</v>
+      </c>
+      <c r="B208" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="B209" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B210" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="20" t="s">
+        <v>329</v>
+      </c>
+      <c r="B211" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="20" t="s">
+        <v>330</v>
+      </c>
+      <c r="B212" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B213" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="B214" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="B215" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="B216" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="B217" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B218" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B219" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B220" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="B221" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B222" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B223" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B224" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="B225" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="B226" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="B227" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="B228" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="20" t="s">
+        <v>347</v>
+      </c>
+      <c r="B229" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="B230" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="B231" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B232" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="B233" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="B234" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="20" t="s">
+        <v>353</v>
+      </c>
+      <c r="B235" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="20" t="s">
+        <v>354</v>
+      </c>
+      <c r="B236" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B237" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="B238" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="20" t="s">
+        <v>357</v>
+      </c>
+      <c r="B239" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B240" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B241" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B242" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B243" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="B244" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="B245" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="B246" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="20" t="s">
+        <v>365</v>
+      </c>
+      <c r="B247" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="B248" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="B249" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="B250" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="B251" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="B252" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="B253" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B254" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="B255" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="B256" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="B257" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="B258" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="20" t="s">
+        <v>377</v>
+      </c>
+      <c r="B259" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="B260" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="20" t="s">
+        <v>379</v>
+      </c>
+      <c r="B261" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="B262" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="B263" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="20" t="s">
+        <v>382</v>
+      </c>
+      <c r="B264" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="20" t="s">
+        <v>383</v>
+      </c>
+      <c r="B265" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="20" t="s">
+        <v>384</v>
+      </c>
+      <c r="B266" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="B267" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="B268" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="B269" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="B270" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2834,7 +4772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>